<commit_message>
Additional updates to try and get this to work across platforms
</commit_message>
<xml_diff>
--- a/Bearstore_Web_App_Project_1/Data_Files/Contact_List.xlsx
+++ b/Bearstore_Web_App_Project_1/Data_Files/Contact_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Shared_TC_Projects\Demo_CI_Suite\Bearstore_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Shared_TC_Projects\TC_Head_Start_Suite\Bearstore_Web_App_Project_1\Data_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC9D242-D0DE-4A6E-A3FB-AE91C2154CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A511CB-8D47-43E3-96A7-DD6746321EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="10920" xr2:uid="{084FFFA1-4D60-4752-B414-257B00A5D176}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{084FFFA1-4D60-4752-B414-257B00A5D176}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact_Information" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -45,101 +45,112 @@
     <t>Enquiry</t>
   </si>
   <si>
-    <t>Shelley Head</t>
-  </si>
-  <si>
-    <t>campos@tortor.edu</t>
-  </si>
-  <si>
-    <t>Help</t>
-  </si>
-  <si>
-    <t>Rogan Anderson</t>
-  </si>
-  <si>
-    <t>lowery@aliquam.us</t>
-  </si>
-  <si>
-    <t>Shipment is missing</t>
-  </si>
-  <si>
     <t>Gil Strong</t>
   </si>
   <si>
-    <t>snow@pulvinar.net</t>
-  </si>
-  <si>
-    <t>Thanks for the fast delivery</t>
-  </si>
-  <si>
     <t>Kasper Nash</t>
   </si>
   <si>
-    <t>dickson@nonummy.net</t>
-  </si>
-  <si>
     <t>Please help with my order</t>
   </si>
   <si>
     <t>Cain Combs</t>
   </si>
   <si>
-    <t>sargent@lorem.gov</t>
-  </si>
-  <si>
     <t>Great Prodcuts</t>
   </si>
   <si>
     <t>Wing Collier</t>
   </si>
   <si>
-    <t>weeks@lacus.org</t>
-  </si>
-  <si>
     <t>Love the prices</t>
   </si>
   <si>
     <t>Diana Shaw</t>
   </si>
   <si>
-    <t>beck@turpis.us</t>
-  </si>
-  <si>
     <t>Is shipping free</t>
   </si>
   <si>
     <t>Elijah Barnett</t>
   </si>
   <si>
-    <t>pickett@quis.us</t>
-  </si>
-  <si>
     <t>Where's my stuff?</t>
   </si>
   <si>
     <t>Herman Crosby</t>
   </si>
   <si>
-    <t>wise@hendrerit.us</t>
-  </si>
-  <si>
     <t>I bought it all</t>
   </si>
   <si>
     <t>Dan Lagomarsino</t>
   </si>
   <si>
-    <t>dan@smartbear.com</t>
+    <t>Help, I've fallen and I cannot get up</t>
+  </si>
+  <si>
+    <t>How can you have any pudding, if you don't eat your meat?</t>
+  </si>
+  <si>
+    <t>Roger Gilmour</t>
+  </si>
+  <si>
+    <t>Sam Power</t>
+  </si>
+  <si>
+    <t>Thanks for the fast delivery, you guys rock!!!</t>
+  </si>
+  <si>
+    <t>Seriously…????</t>
+  </si>
+  <si>
+    <t>SamPower@Null.Org</t>
+  </si>
+  <si>
+    <t>RogerGilmour@Null.Org</t>
+  </si>
+  <si>
+    <t>DanLagomarsino@Null.Org</t>
+  </si>
+  <si>
+    <t>GilStrong@Null.org</t>
+  </si>
+  <si>
+    <t>KasperNash@Null.org</t>
+  </si>
+  <si>
+    <t>CainCombs@Null.org</t>
+  </si>
+  <si>
+    <t>WingCollier@Null.org</t>
+  </si>
+  <si>
+    <t>DianaShaw@Null.org</t>
+  </si>
+  <si>
+    <t>ElijahBarnett@Null.org</t>
+  </si>
+  <si>
+    <t>HermanCrosby@Null.org</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -162,14 +173,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -485,14 +499,14 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -508,115 +522,127 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>19</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>16</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{B223B0AF-7CAA-4F25-8B48-10B162FFFC94}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{0CDAF89F-7E62-49F0-88B2-BC13880FBF01}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{864E3579-3E6C-4E55-9252-614CE5A12310}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{029B8EC5-03CA-45AC-A1A3-F8B7FA051643}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{87F96320-2CB5-4BCE-97AC-AB6FDF3A8BEC}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{60076C8A-B3CF-4990-88AE-613687E2C3CC}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{A2B3E3B5-6C29-4B42-8949-2E1885C98B66}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{03C33D6F-8571-4F3B-B064-6E3F7EA5F8BD}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{0BF73830-74FD-4E81-8AD4-811C33FBEB3C}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{AB6F4C26-1CE1-480A-8477-FE877146D784}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Data_Files and related test module
</commit_message>
<xml_diff>
--- a/Bearstore_Web_App_Project_1/Data_Files/Contact_List.xlsx
+++ b/Bearstore_Web_App_Project_1/Data_Files/Contact_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Shared_TC_Projects\TC_Head_Start_Suite\Bearstore_Web_App_Project_1\Data_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A511CB-8D47-43E3-96A7-DD6746321EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF10DC5-2B16-41FB-83E9-00CA51DF558B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{084FFFA1-4D60-4752-B414-257B00A5D176}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{084FFFA1-4D60-4752-B414-257B00A5D176}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact_Information" sheetId="1" r:id="rId1"/>
@@ -51,27 +51,15 @@
     <t>Kasper Nash</t>
   </si>
   <si>
-    <t>Please help with my order</t>
-  </si>
-  <si>
     <t>Cain Combs</t>
   </si>
   <si>
-    <t>Great Prodcuts</t>
-  </si>
-  <si>
     <t>Wing Collier</t>
   </si>
   <si>
-    <t>Love the prices</t>
-  </si>
-  <si>
     <t>Diana Shaw</t>
   </si>
   <si>
-    <t>Is shipping free</t>
-  </si>
-  <si>
     <t>Elijah Barnett</t>
   </si>
   <si>
@@ -81,15 +69,9 @@
     <t>Herman Crosby</t>
   </si>
   <si>
-    <t>I bought it all</t>
-  </si>
-  <si>
     <t>Dan Lagomarsino</t>
   </si>
   <si>
-    <t>Help, I've fallen and I cannot get up</t>
-  </si>
-  <si>
     <t>How can you have any pudding, if you don't eat your meat?</t>
   </si>
   <si>
@@ -102,9 +84,6 @@
     <t>Thanks for the fast delivery, you guys rock!!!</t>
   </si>
   <si>
-    <t>Seriously…????</t>
-  </si>
-  <si>
     <t>SamPower@Null.Org</t>
   </si>
   <si>
@@ -133,6 +112,27 @@
   </si>
   <si>
     <t>HermanCrosby@Null.org</t>
+  </si>
+  <si>
+    <t>Help, I've fallen and I cannot get up!</t>
+  </si>
+  <si>
+    <t>Please help with my order.</t>
+  </si>
+  <si>
+    <t>Great Products!</t>
+  </si>
+  <si>
+    <t>Love the prices!</t>
+  </si>
+  <si>
+    <t>Is shipping free?</t>
+  </si>
+  <si>
+    <t>Seriously?</t>
+  </si>
+  <si>
+    <t>I bought it all!!!</t>
   </si>
 </sst>
 </file>
@@ -499,7 +499,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,24 +522,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -547,10 +547,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -558,76 +558,76 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>